<commit_message>
seems to work for xlsx & xls
</commit_message>
<xml_diff>
--- a/test/fixtures/files/test_excel_simplefilecontent.xlsx
+++ b/test/fixtures/files/test_excel_simplefilecontent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="4580" windowWidth="10220" windowHeight="7060" tabRatio="500"/>
+    <workbookView xWindow="8800" yWindow="4580" windowWidth="19700" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>